<commit_message>
updated data preparation (added contingency table related data) and fixed decline effect plot
</commit_message>
<xml_diff>
--- a/data/input/data_extraction_UnpublishedThesis.xlsx
+++ b/data/input/data_extraction_UnpublishedThesis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyadimri/Library/CloudStorage/Dropbox/GitHub_Repo/test_junk/GNM/data/02_data_extraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyadimri/Library/CloudStorage/Dropbox/GitHub_Repo/GNM_Analysis/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B336723F-D7B0-A142-AFC2-BC542776E4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1707FC-275C-2A47-A1D4-787E0A320B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33220" yWindow="500" windowWidth="43580" windowHeight="21100" xr2:uid="{2338411D-A035-6640-9B5F-097AD98E903E}"/>
   </bookViews>
@@ -399,9 +399,6 @@
     </r>
   </si>
   <si>
-    <t>check</t>
-  </si>
-  <si>
     <t>include</t>
   </si>
   <si>
@@ -472,6 +469,9 @@
   </si>
   <si>
     <t>shared_control</t>
+  </si>
+  <si>
+    <t>contingency table</t>
   </si>
 </sst>
 </file>
@@ -919,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DCDDD25-569C-114E-BA1C-CFE63559CC31}">
   <dimension ref="A1:AX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="AW1" sqref="AW1:AX1"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1123,15 +1123,15 @@
         <v>79</v>
       </c>
       <c r="AW1" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="AX1" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="AX1" s="6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:50" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>85</v>
@@ -1143,31 +1143,31 @@
         <v>108</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" t="s">
         <v>109</v>
       </c>
       <c r="G2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" t="s">
         <v>120</v>
       </c>
-      <c r="L2" t="s">
-        <v>121</v>
-      </c>
       <c r="M2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -1188,7 +1188,7 @@
         <v>1.08</v>
       </c>
       <c r="T2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U2">
         <v>9</v>
@@ -1203,58 +1203,58 @@
         <v>0.93</v>
       </c>
       <c r="Y2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z2">
         <v>9</v>
       </c>
       <c r="AA2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB2" t="s">
         <v>123</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO2" t="s">
         <v>124</v>
       </c>
-      <c r="AC2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE2">
-        <v>1</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>125</v>
-      </c>
       <c r="AP2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ2" t="s">
         <v>85</v>
@@ -1266,13 +1266,13 @@
         <v>85</v>
       </c>
       <c r="AT2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AU2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AV2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AW2">
         <v>1</v>
@@ -1283,7 +1283,7 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
         <v>85</v>
@@ -1295,31 +1295,31 @@
         <v>108</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
         <v>109</v>
       </c>
       <c r="G3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" t="s">
         <v>120</v>
       </c>
-      <c r="L3" t="s">
-        <v>121</v>
-      </c>
       <c r="M3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -1340,7 +1340,7 @@
         <v>1.28</v>
       </c>
       <c r="T3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U3">
         <v>9</v>
@@ -1355,58 +1355,58 @@
         <v>1.18</v>
       </c>
       <c r="Y3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z3">
         <v>9</v>
       </c>
       <c r="AA3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AB3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO3" t="s">
         <v>124</v>
       </c>
-      <c r="AC3" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE3">
-        <v>1</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>125</v>
-      </c>
       <c r="AP3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ3" t="s">
         <v>85</v>
@@ -1418,13 +1418,13 @@
         <v>85</v>
       </c>
       <c r="AT3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AU3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AV3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AW3">
         <v>1</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
         <v>85</v>
@@ -1447,31 +1447,31 @@
         <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F4" t="s">
         <v>109</v>
       </c>
       <c r="G4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" t="s">
         <v>120</v>
       </c>
-      <c r="L4" t="s">
-        <v>121</v>
-      </c>
       <c r="M4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -1492,7 +1492,7 @@
         <v>1.53</v>
       </c>
       <c r="T4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U4">
         <v>8</v>
@@ -1507,58 +1507,58 @@
         <v>1.06</v>
       </c>
       <c r="Y4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z4">
         <v>9</v>
       </c>
       <c r="AA4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AB4" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE4">
+        <v>1</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO4" t="s">
         <v>124</v>
       </c>
-      <c r="AC4" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE4">
-        <v>1</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>125</v>
-      </c>
       <c r="AP4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ4" t="s">
         <v>85</v>
@@ -1570,13 +1570,13 @@
         <v>85</v>
       </c>
       <c r="AT4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AU4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AV4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AW4">
         <v>1</v>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
         <v>85</v>
@@ -1599,31 +1599,31 @@
         <v>108</v>
       </c>
       <c r="E5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F5" t="s">
         <v>109</v>
       </c>
       <c r="G5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="11" t="s">
+      <c r="L5" t="s">
         <v>120</v>
       </c>
-      <c r="L5" t="s">
-        <v>121</v>
-      </c>
       <c r="M5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -1644,7 +1644,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="T5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U5">
         <v>8</v>
@@ -1659,58 +1659,58 @@
         <v>1.33</v>
       </c>
       <c r="Y5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z5">
         <v>7</v>
       </c>
       <c r="AA5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AB5" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO5" t="s">
         <v>124</v>
       </c>
-      <c r="AC5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE5">
-        <v>1</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>125</v>
-      </c>
       <c r="AP5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ5" t="s">
         <v>85</v>
@@ -1722,13 +1722,13 @@
         <v>85</v>
       </c>
       <c r="AT5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AU5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AV5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AW5">
         <v>1</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
         <v>85</v>
@@ -1751,31 +1751,31 @@
         <v>108</v>
       </c>
       <c r="E6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6" t="s">
         <v>109</v>
       </c>
       <c r="G6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6" s="11" t="s">
+      <c r="L6" t="s">
         <v>120</v>
       </c>
-      <c r="L6" t="s">
-        <v>121</v>
-      </c>
       <c r="M6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -1796,7 +1796,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="T6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U6">
         <v>6</v>
@@ -1811,58 +1811,58 @@
         <v>1.04</v>
       </c>
       <c r="Y6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z6">
         <v>6</v>
       </c>
       <c r="AA6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AB6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO6" t="s">
         <v>124</v>
       </c>
-      <c r="AC6" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE6">
-        <v>1</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>125</v>
-      </c>
       <c r="AP6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ6" t="s">
         <v>85</v>
@@ -1874,13 +1874,13 @@
         <v>85</v>
       </c>
       <c r="AT6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AU6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AV6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AW6">
         <v>1</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
         <v>85</v>
@@ -1903,31 +1903,31 @@
         <v>108</v>
       </c>
       <c r="E7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F7" t="s">
         <v>109</v>
       </c>
       <c r="G7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7" s="11" t="s">
+      <c r="L7" t="s">
         <v>120</v>
       </c>
-      <c r="L7" t="s">
-        <v>121</v>
-      </c>
       <c r="M7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -1948,7 +1948,7 @@
         <v>0.97</v>
       </c>
       <c r="T7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U7">
         <v>6</v>
@@ -1963,58 +1963,58 @@
         <v>0.92</v>
       </c>
       <c r="Y7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z7">
         <v>6</v>
       </c>
       <c r="AA7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AB7" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>113</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO7" t="s">
         <v>124</v>
       </c>
-      <c r="AC7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE7">
-        <v>1</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>125</v>
-      </c>
       <c r="AP7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ7" t="s">
         <v>85</v>
@@ -2026,13 +2026,13 @@
         <v>85</v>
       </c>
       <c r="AT7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AU7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AV7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AW7">
         <v>1</v>
@@ -2043,7 +2043,7 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
         <v>85</v>
@@ -2055,31 +2055,31 @@
         <v>108</v>
       </c>
       <c r="E8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
         <v>109</v>
       </c>
       <c r="G8" t="s">
+        <v>118</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8" s="11" t="s">
+      <c r="L8" t="s">
         <v>120</v>
       </c>
-      <c r="L8" t="s">
-        <v>121</v>
-      </c>
       <c r="M8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -2100,7 +2100,7 @@
         <v>0.34</v>
       </c>
       <c r="T8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U8">
         <v>4</v>
@@ -2115,58 +2115,58 @@
         <v>0.69</v>
       </c>
       <c r="Y8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z8">
         <v>5</v>
       </c>
       <c r="AA8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AB8" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>113</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO8" t="s">
         <v>124</v>
       </c>
-      <c r="AC8" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE8">
-        <v>1</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>125</v>
-      </c>
       <c r="AP8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ8" t="s">
         <v>85</v>
@@ -2178,13 +2178,13 @@
         <v>85</v>
       </c>
       <c r="AT8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AU8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AV8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AW8">
         <v>1</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
         <v>85</v>
@@ -2207,31 +2207,31 @@
         <v>108</v>
       </c>
       <c r="E9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F9" t="s">
         <v>109</v>
       </c>
       <c r="G9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9" s="11" t="s">
+      <c r="L9" t="s">
         <v>120</v>
       </c>
-      <c r="L9" t="s">
-        <v>121</v>
-      </c>
       <c r="M9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -2252,7 +2252,7 @@
         <v>85</v>
       </c>
       <c r="T9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U9">
         <v>9</v>
@@ -2267,19 +2267,19 @@
         <v>85</v>
       </c>
       <c r="Y9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z9">
         <v>9</v>
       </c>
       <c r="AA9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AC9" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="AD9" t="s">
         <v>85</v>
@@ -2309,16 +2309,16 @@
         <v>85</v>
       </c>
       <c r="AM9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AN9" t="s">
         <v>85</v>
       </c>
       <c r="AO9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AP9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ9" t="s">
         <v>85</v>
@@ -2330,13 +2330,13 @@
         <v>85</v>
       </c>
       <c r="AT9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AU9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AV9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AW9">
         <v>1</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
         <v>85</v>
@@ -2359,31 +2359,31 @@
         <v>108</v>
       </c>
       <c r="E10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F10" t="s">
         <v>109</v>
       </c>
       <c r="G10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10" s="11" t="s">
+      <c r="L10" t="s">
         <v>120</v>
       </c>
-      <c r="L10" t="s">
-        <v>121</v>
-      </c>
       <c r="M10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -2404,7 +2404,7 @@
         <v>43.88</v>
       </c>
       <c r="T10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U10">
         <v>9</v>
@@ -2419,58 +2419,58 @@
         <v>38.39</v>
       </c>
       <c r="Y10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z10">
         <v>9</v>
       </c>
       <c r="AA10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB10" t="s">
         <v>133</v>
       </c>
-      <c r="AB10" t="s">
-        <v>134</v>
-      </c>
       <c r="AC10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE10">
+        <v>1</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM10" t="s">
         <v>113</v>
       </c>
-      <c r="AD10" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE10">
-        <v>1</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK10" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL10" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM10" t="s">
-        <v>114</v>
-      </c>
       <c r="AN10" t="s">
         <v>85</v>
       </c>
       <c r="AO10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AP10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ10" t="s">
         <v>85</v>
@@ -2482,13 +2482,13 @@
         <v>85</v>
       </c>
       <c r="AT10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AU10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AV10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AW10">
         <v>1</v>

</xml_diff>